<commit_message>
added different gwp types and some extra mappings in new esto data
</commit_message>
<xml_diff>
--- a/config/aperc_to_ipcc_sector_mappings.xlsx
+++ b/config/aperc_to_ipcc_sector_mappings.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7024" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7044" uniqueCount="241">
   <si>
     <t>aperc_sector</t>
   </si>
@@ -4324,7 +4324,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D333"/>
+  <dimension ref="A1:D338"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8990,6 +8990,76 @@
       </c>
       <c r="D333" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4">
+      <c r="A334" t="s">
+        <v>161</v>
+      </c>
+      <c r="B334" t="s">
+        <v>39</v>
+      </c>
+      <c r="C334" t="s">
+        <v>53</v>
+      </c>
+      <c r="D334" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4">
+      <c r="A335" t="s">
+        <v>150</v>
+      </c>
+      <c r="B335" t="s">
+        <v>30</v>
+      </c>
+      <c r="C335" t="s">
+        <v>53</v>
+      </c>
+      <c r="D335" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4">
+      <c r="A336" t="s">
+        <v>150</v>
+      </c>
+      <c r="B336" t="s">
+        <v>31</v>
+      </c>
+      <c r="C336" t="s">
+        <v>53</v>
+      </c>
+      <c r="D336" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4">
+      <c r="A337" t="s">
+        <v>162</v>
+      </c>
+      <c r="B337" t="s">
+        <v>40</v>
+      </c>
+      <c r="C337" t="s">
+        <v>53</v>
+      </c>
+      <c r="D337" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4">
+      <c r="A338" t="s">
+        <v>159</v>
+      </c>
+      <c r="B338" t="s">
+        <v>84</v>
+      </c>
+      <c r="C338" t="s">
+        <v>53</v>
+      </c>
+      <c r="D338" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added transfers subsector to not_applicable_sectors_broad_categories
</commit_message>
<xml_diff>
--- a/config/aperc_to_ipcc_sector_mappings.xlsx
+++ b/config/aperc_to_ipcc_sector_mappings.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6360" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6364" uniqueCount="218">
   <si>
     <t>aperc_sector</t>
   </si>
@@ -4255,7 +4255,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D168"/>
+  <dimension ref="A1:D169"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6611,6 +6611,20 @@
       </c>
       <c r="D168" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169" t="s">
+        <v>151</v>
+      </c>
+      <c r="B169" t="s">
+        <v>85</v>
+      </c>
+      <c r="C169" t="s">
+        <v>53</v>
+      </c>
+      <c r="D169" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
input data name change
</commit_message>
<xml_diff>
--- a/config/aperc_to_ipcc_sector_mappings.xlsx
+++ b/config/aperc_to_ipcc_sector_mappings.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6360" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6368" uniqueCount="218">
   <si>
     <t>aperc_sector</t>
   </si>
@@ -4255,7 +4255,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D168"/>
+  <dimension ref="A1:D169"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6611,6 +6611,20 @@
       </c>
       <c r="D168" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169" t="s">
+        <v>151</v>
+      </c>
+      <c r="B169" t="s">
+        <v>85</v>
+      </c>
+      <c r="C169" t="s">
+        <v>53</v>
+      </c>
+      <c r="D169" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -15008,7 +15022,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D553"/>
+  <dimension ref="A1:D554"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -21535,7 +21549,7 @@
         <v>129</v>
       </c>
       <c r="D466" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="467" spans="1:4">
@@ -21543,13 +21557,13 @@
         <v>125</v>
       </c>
       <c r="B467" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C467" t="s">
         <v>129</v>
       </c>
       <c r="D467" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="468" spans="1:4">
@@ -21557,13 +21571,13 @@
         <v>125</v>
       </c>
       <c r="B468" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C468" t="s">
         <v>129</v>
       </c>
       <c r="D468" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="469" spans="1:4">
@@ -21571,13 +21585,13 @@
         <v>125</v>
       </c>
       <c r="B469" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C469" t="s">
         <v>129</v>
       </c>
       <c r="D469" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="470" spans="1:4">
@@ -21585,13 +21599,13 @@
         <v>125</v>
       </c>
       <c r="B470" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C470" t="s">
         <v>129</v>
       </c>
       <c r="D470" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="471" spans="1:4">
@@ -21599,13 +21613,13 @@
         <v>125</v>
       </c>
       <c r="B471" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="C471" t="s">
         <v>129</v>
       </c>
       <c r="D471" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
     </row>
     <row r="472" spans="1:4">
@@ -21613,27 +21627,27 @@
         <v>125</v>
       </c>
       <c r="B472" t="s">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="C472" t="s">
         <v>129</v>
       </c>
       <c r="D472" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="473" spans="1:4">
       <c r="A473" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B473" t="s">
-        <v>29</v>
+        <v>95</v>
       </c>
       <c r="C473" t="s">
         <v>129</v>
       </c>
       <c r="D473" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
     </row>
     <row r="474" spans="1:4">
@@ -21641,13 +21655,13 @@
         <v>126</v>
       </c>
       <c r="B474" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C474" t="s">
         <v>129</v>
       </c>
       <c r="D474" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="475" spans="1:4">
@@ -21655,7 +21669,7 @@
         <v>126</v>
       </c>
       <c r="B475" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C475" t="s">
         <v>129</v>
@@ -21669,13 +21683,13 @@
         <v>126</v>
       </c>
       <c r="B476" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C476" t="s">
         <v>129</v>
       </c>
       <c r="D476" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="477" spans="1:4">
@@ -21683,13 +21697,13 @@
         <v>126</v>
       </c>
       <c r="B477" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C477" t="s">
         <v>129</v>
       </c>
       <c r="D477" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="478" spans="1:4">
@@ -21697,13 +21711,13 @@
         <v>126</v>
       </c>
       <c r="B478" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C478" t="s">
         <v>129</v>
       </c>
       <c r="D478" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="479" spans="1:4">
@@ -21711,13 +21725,13 @@
         <v>126</v>
       </c>
       <c r="B479" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C479" t="s">
         <v>129</v>
       </c>
       <c r="D479" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="480" spans="1:4">
@@ -21725,18 +21739,18 @@
         <v>126</v>
       </c>
       <c r="B480" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="C480" t="s">
         <v>129</v>
       </c>
       <c r="D480" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
     </row>
     <row r="481" spans="1:4">
       <c r="A481" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="B481" t="s">
         <v>91</v>
@@ -21750,16 +21764,16 @@
     </row>
     <row r="482" spans="1:4">
       <c r="A482" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="B482" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
       <c r="C482" t="s">
         <v>129</v>
       </c>
       <c r="D482" t="s">
-        <v>59</v>
+        <v>104</v>
       </c>
     </row>
     <row r="483" spans="1:4">
@@ -21767,13 +21781,13 @@
         <v>127</v>
       </c>
       <c r="B483" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C483" t="s">
         <v>129</v>
       </c>
       <c r="D483" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="484" spans="1:4">
@@ -21781,7 +21795,7 @@
         <v>127</v>
       </c>
       <c r="B484" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C484" t="s">
         <v>129</v>
@@ -21795,13 +21809,13 @@
         <v>127</v>
       </c>
       <c r="B485" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C485" t="s">
         <v>129</v>
       </c>
       <c r="D485" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="486" spans="1:4">
@@ -21809,13 +21823,13 @@
         <v>127</v>
       </c>
       <c r="B486" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C486" t="s">
         <v>129</v>
       </c>
       <c r="D486" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="487" spans="1:4">
@@ -21823,13 +21837,13 @@
         <v>127</v>
       </c>
       <c r="B487" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C487" t="s">
         <v>129</v>
       </c>
       <c r="D487" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="488" spans="1:4">
@@ -21837,13 +21851,13 @@
         <v>127</v>
       </c>
       <c r="B488" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C488" t="s">
         <v>129</v>
       </c>
       <c r="D488" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="489" spans="1:4">
@@ -21851,27 +21865,27 @@
         <v>127</v>
       </c>
       <c r="B489" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="C489" t="s">
         <v>129</v>
       </c>
       <c r="D489" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
     </row>
     <row r="490" spans="1:4">
       <c r="A490" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B490" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
       <c r="C490" t="s">
         <v>129</v>
       </c>
       <c r="D490" t="s">
-        <v>59</v>
+        <v>104</v>
       </c>
     </row>
     <row r="491" spans="1:4">
@@ -21879,13 +21893,13 @@
         <v>128</v>
       </c>
       <c r="B491" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C491" t="s">
         <v>129</v>
       </c>
       <c r="D491" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="492" spans="1:4">
@@ -21893,7 +21907,7 @@
         <v>128</v>
       </c>
       <c r="B492" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C492" t="s">
         <v>129</v>
@@ -21907,13 +21921,13 @@
         <v>128</v>
       </c>
       <c r="B493" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C493" t="s">
         <v>129</v>
       </c>
       <c r="D493" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="494" spans="1:4">
@@ -21921,13 +21935,13 @@
         <v>128</v>
       </c>
       <c r="B494" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C494" t="s">
         <v>129</v>
       </c>
       <c r="D494" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="495" spans="1:4">
@@ -21935,7 +21949,7 @@
         <v>128</v>
       </c>
       <c r="B495" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C495" t="s">
         <v>129</v>
@@ -21949,13 +21963,13 @@
         <v>128</v>
       </c>
       <c r="B496" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C496" t="s">
         <v>129</v>
       </c>
       <c r="D496" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="497" spans="1:4">
@@ -21963,13 +21977,13 @@
         <v>128</v>
       </c>
       <c r="B497" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C497" t="s">
         <v>129</v>
       </c>
       <c r="D497" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="498" spans="1:4">
@@ -21977,13 +21991,13 @@
         <v>128</v>
       </c>
       <c r="B498" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C498" t="s">
         <v>129</v>
       </c>
       <c r="D498" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="499" spans="1:4">
@@ -21991,13 +22005,13 @@
         <v>128</v>
       </c>
       <c r="B499" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C499" t="s">
         <v>129</v>
       </c>
       <c r="D499" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="500" spans="1:4">
@@ -22005,13 +22019,13 @@
         <v>128</v>
       </c>
       <c r="B500" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C500" t="s">
         <v>129</v>
       </c>
       <c r="D500" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="501" spans="1:4">
@@ -22019,13 +22033,13 @@
         <v>128</v>
       </c>
       <c r="B501" t="s">
-        <v>82</v>
+        <v>40</v>
       </c>
       <c r="C501" t="s">
         <v>129</v>
       </c>
       <c r="D501" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
     </row>
     <row r="502" spans="1:4">
@@ -22033,13 +22047,13 @@
         <v>128</v>
       </c>
       <c r="B502" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="C502" t="s">
         <v>129</v>
       </c>
       <c r="D502" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
     </row>
     <row r="503" spans="1:4">
@@ -22047,7 +22061,7 @@
         <v>128</v>
       </c>
       <c r="B503" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C503" t="s">
         <v>129</v>
@@ -22061,13 +22075,13 @@
         <v>128</v>
       </c>
       <c r="B504" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C504" t="s">
         <v>129</v>
       </c>
       <c r="D504" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="505" spans="1:4">
@@ -22075,13 +22089,13 @@
         <v>128</v>
       </c>
       <c r="B505" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C505" t="s">
         <v>129</v>
       </c>
       <c r="D505" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="506" spans="1:4">
@@ -22089,13 +22103,13 @@
         <v>128</v>
       </c>
       <c r="B506" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C506" t="s">
         <v>129</v>
       </c>
       <c r="D506" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="507" spans="1:4">
@@ -22103,13 +22117,13 @@
         <v>128</v>
       </c>
       <c r="B507" t="s">
-        <v>85</v>
+        <v>46</v>
       </c>
       <c r="C507" t="s">
         <v>129</v>
       </c>
       <c r="D507" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
     </row>
     <row r="508" spans="1:4">
@@ -22117,13 +22131,13 @@
         <v>128</v>
       </c>
       <c r="B508" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C508" t="s">
         <v>129</v>
       </c>
       <c r="D508" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="509" spans="1:4">
@@ -22131,7 +22145,7 @@
         <v>128</v>
       </c>
       <c r="B509" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C509" t="s">
         <v>129</v>
@@ -22145,13 +22159,13 @@
         <v>128</v>
       </c>
       <c r="B510" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C510" t="s">
         <v>129</v>
       </c>
       <c r="D510" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="511" spans="1:4">
@@ -22159,13 +22173,13 @@
         <v>128</v>
       </c>
       <c r="B511" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C511" t="s">
         <v>129</v>
       </c>
       <c r="D511" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="512" spans="1:4">
@@ -22173,13 +22187,13 @@
         <v>128</v>
       </c>
       <c r="B512" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C512" t="s">
         <v>129</v>
       </c>
       <c r="D512" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="513" spans="1:4">
@@ -22187,32 +22201,32 @@
         <v>128</v>
       </c>
       <c r="B513" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
       <c r="C513" t="s">
         <v>129</v>
       </c>
       <c r="D513" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
     </row>
     <row r="514" spans="1:4">
       <c r="A514" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="B514" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="C514" t="s">
         <v>129</v>
       </c>
       <c r="D514" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
     </row>
     <row r="515" spans="1:4">
       <c r="A515" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B515" t="s">
         <v>91</v>
@@ -22226,30 +22240,30 @@
     </row>
     <row r="516" spans="1:4">
       <c r="A516" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B516" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C516" t="s">
         <v>129</v>
       </c>
       <c r="D516" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="517" spans="1:4">
       <c r="A517" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="B517" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="C517" t="s">
         <v>129</v>
       </c>
       <c r="D517" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
     </row>
     <row r="518" spans="1:4">
@@ -22257,13 +22271,13 @@
         <v>108</v>
       </c>
       <c r="B518" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="C518" t="s">
         <v>129</v>
       </c>
       <c r="D518" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="519" spans="1:4">
@@ -22271,13 +22285,13 @@
         <v>108</v>
       </c>
       <c r="B519" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C519" t="s">
         <v>129</v>
       </c>
       <c r="D519" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="520" spans="1:4">
@@ -22285,13 +22299,13 @@
         <v>108</v>
       </c>
       <c r="B520" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C520" t="s">
         <v>129</v>
       </c>
       <c r="D520" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="521" spans="1:4">
@@ -22299,41 +22313,41 @@
         <v>108</v>
       </c>
       <c r="B521" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C521" t="s">
         <v>129</v>
       </c>
       <c r="D521" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="522" spans="1:4">
       <c r="A522" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B522" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C522" t="s">
         <v>129</v>
       </c>
       <c r="D522" t="s">
-        <v>61</v>
+        <v>107</v>
       </c>
     </row>
     <row r="523" spans="1:4">
       <c r="A523" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="B523" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="C523" t="s">
         <v>129</v>
       </c>
       <c r="D523" t="s">
-        <v>146</v>
+        <v>61</v>
       </c>
     </row>
     <row r="524" spans="1:4">
@@ -22341,27 +22355,27 @@
         <v>125</v>
       </c>
       <c r="B524" t="s">
-        <v>87</v>
+        <v>41</v>
       </c>
       <c r="C524" t="s">
         <v>129</v>
       </c>
       <c r="D524" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
     </row>
     <row r="525" spans="1:4">
       <c r="A525" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="B525" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="C525" t="s">
         <v>129</v>
       </c>
       <c r="D525" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
     </row>
     <row r="526" spans="1:4">
@@ -22369,13 +22383,13 @@
         <v>111</v>
       </c>
       <c r="B526" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C526" t="s">
         <v>129</v>
       </c>
       <c r="D526" t="s">
-        <v>146</v>
+        <v>75</v>
       </c>
     </row>
     <row r="527" spans="1:4">
@@ -22383,13 +22397,13 @@
         <v>111</v>
       </c>
       <c r="B527" t="s">
-        <v>87</v>
+        <v>41</v>
       </c>
       <c r="C527" t="s">
         <v>129</v>
       </c>
       <c r="D527" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
     </row>
     <row r="528" spans="1:4">
@@ -22397,27 +22411,27 @@
         <v>111</v>
       </c>
       <c r="B528" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C528" t="s">
         <v>129</v>
       </c>
       <c r="D528" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="529" spans="1:4">
       <c r="A529" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B529" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="C529" t="s">
         <v>129</v>
       </c>
       <c r="D529" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
     </row>
     <row r="530" spans="1:4">
@@ -22425,41 +22439,41 @@
         <v>112</v>
       </c>
       <c r="B530" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C530" t="s">
         <v>129</v>
       </c>
       <c r="D530" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
     </row>
     <row r="531" spans="1:4">
       <c r="A531" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B531" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C531" t="s">
         <v>129</v>
       </c>
       <c r="D531" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="532" spans="1:4">
       <c r="A532" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B532" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="C532" t="s">
         <v>129</v>
       </c>
       <c r="D532" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
     </row>
     <row r="533" spans="1:4">
@@ -22467,27 +22481,27 @@
         <v>114</v>
       </c>
       <c r="B533" t="s">
-        <v>92</v>
+        <v>27</v>
       </c>
       <c r="C533" t="s">
         <v>129</v>
       </c>
       <c r="D533" t="s">
-        <v>105</v>
+        <v>56</v>
       </c>
     </row>
     <row r="534" spans="1:4">
       <c r="A534" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B534" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="C534" t="s">
         <v>129</v>
       </c>
       <c r="D534" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
     </row>
     <row r="535" spans="1:4">
@@ -22495,27 +22509,27 @@
         <v>115</v>
       </c>
       <c r="B535" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C535" t="s">
         <v>129</v>
       </c>
       <c r="D535" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
     </row>
     <row r="536" spans="1:4">
       <c r="A536" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B536" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C536" t="s">
         <v>129</v>
       </c>
       <c r="D536" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="537" spans="1:4">
@@ -22523,13 +22537,13 @@
         <v>109</v>
       </c>
       <c r="B537" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C537" t="s">
         <v>129</v>
       </c>
       <c r="D537" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
     </row>
     <row r="538" spans="1:4">
@@ -22537,41 +22551,41 @@
         <v>109</v>
       </c>
       <c r="B538" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C538" t="s">
         <v>129</v>
       </c>
       <c r="D538" t="s">
-        <v>102</v>
+        <v>61</v>
       </c>
     </row>
     <row r="539" spans="1:4">
       <c r="A539" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B539" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C539" t="s">
         <v>129</v>
       </c>
       <c r="D539" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="540" spans="1:4">
       <c r="A540" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B540" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="C540" t="s">
         <v>129</v>
       </c>
       <c r="D540" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
     </row>
     <row r="541" spans="1:4">
@@ -22579,27 +22593,27 @@
         <v>117</v>
       </c>
       <c r="B541" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C541" t="s">
         <v>129</v>
       </c>
       <c r="D541" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
     </row>
     <row r="542" spans="1:4">
       <c r="A542" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B542" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C542" t="s">
         <v>129</v>
       </c>
       <c r="D542" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="543" spans="1:4">
@@ -22607,13 +22621,13 @@
         <v>118</v>
       </c>
       <c r="B543" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="C543" t="s">
         <v>129</v>
       </c>
       <c r="D543" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="544" spans="1:4">
@@ -22621,13 +22635,13 @@
         <v>118</v>
       </c>
       <c r="B544" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C544" t="s">
         <v>129</v>
       </c>
       <c r="D544" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="545" spans="1:4">
@@ -22635,27 +22649,27 @@
         <v>118</v>
       </c>
       <c r="B545" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C545" t="s">
         <v>129</v>
       </c>
       <c r="D545" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="546" spans="1:4">
       <c r="A546" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B546" t="s">
-        <v>50</v>
+        <v>94</v>
       </c>
       <c r="C546" t="s">
         <v>129</v>
       </c>
       <c r="D546" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
     </row>
     <row r="547" spans="1:4">
@@ -22663,27 +22677,27 @@
         <v>119</v>
       </c>
       <c r="B547" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C547" t="s">
         <v>129</v>
       </c>
       <c r="D547" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
     </row>
     <row r="548" spans="1:4">
       <c r="A548" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B548" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C548" t="s">
         <v>129</v>
       </c>
       <c r="D548" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="549" spans="1:4">
@@ -22691,13 +22705,13 @@
         <v>120</v>
       </c>
       <c r="B549" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C549" t="s">
         <v>129</v>
       </c>
       <c r="D549" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
     </row>
     <row r="550" spans="1:4">
@@ -22705,27 +22719,27 @@
         <v>120</v>
       </c>
       <c r="B550" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C550" t="s">
         <v>129</v>
       </c>
       <c r="D550" t="s">
-        <v>103</v>
+        <v>61</v>
       </c>
     </row>
     <row r="551" spans="1:4">
       <c r="A551" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B551" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="C551" t="s">
         <v>129</v>
       </c>
       <c r="D551" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
     </row>
     <row r="552" spans="1:4">
@@ -22733,13 +22747,13 @@
         <v>121</v>
       </c>
       <c r="B552" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C552" t="s">
         <v>129</v>
       </c>
       <c r="D552" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
     </row>
     <row r="553" spans="1:4">
@@ -22747,12 +22761,26 @@
         <v>121</v>
       </c>
       <c r="B553" t="s">
+        <v>80</v>
+      </c>
+      <c r="C553" t="s">
+        <v>129</v>
+      </c>
+      <c r="D553" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="554" spans="1:4">
+      <c r="A554" t="s">
+        <v>121</v>
+      </c>
+      <c r="B554" t="s">
         <v>88</v>
       </c>
-      <c r="C553" t="s">
-        <v>129</v>
-      </c>
-      <c r="D553" t="s">
+      <c r="C554" t="s">
+        <v>129</v>
+      </c>
+      <c r="D554" t="s">
         <v>103</v>
       </c>
     </row>

</xml_diff>

<commit_message>
provided missing mappings for lng
</commit_message>
<xml_diff>
--- a/config/aperc_to_ipcc_sector_mappings.xlsx
+++ b/config/aperc_to_ipcc_sector_mappings.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6376" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6386" uniqueCount="218">
   <si>
     <t>aperc_sector</t>
   </si>
@@ -13064,7 +13064,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -14393,6 +14393,40 @@
         <v>72</v>
       </c>
       <c r="E78" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>20</v>
+      </c>
+      <c r="B79" t="s">
+        <v>51</v>
+      </c>
+      <c r="C79" t="s">
+        <v>54</v>
+      </c>
+      <c r="D79" t="s">
+        <v>72</v>
+      </c>
+      <c r="E79" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>21</v>
+      </c>
+      <c r="B80" t="s">
+        <v>51</v>
+      </c>
+      <c r="C80" t="s">
+        <v>54</v>
+      </c>
+      <c r="D80" t="s">
+        <v>72</v>
+      </c>
+      <c r="E80" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>